<commit_message>
Great!! Data provider tests are running in parallel.
</commit_message>
<xml_diff>
--- a/resources/testdata.xlsx
+++ b/resources/testdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -90,6 +90,24 @@
   </si>
   <si>
     <t>Mr Akash Sharma</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Shanghai, CN - Pudong (PVG)</t>
+  </si>
+  <si>
+    <t>2/12/2017</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>testUser2@gmail.com</t>
+  </si>
+  <si>
+    <t>1/Jan/1993</t>
   </si>
 </sst>
 </file>
@@ -142,8 +160,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -452,14 +498,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
@@ -540,6 +587,44 @@
         <v>20</v>
       </c>
     </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3">
+        <v>987654321</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3">
+        <v>987654321</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added a test case to test filters.
</commit_message>
<xml_diff>
--- a/resources/testdata.xlsx
+++ b/resources/testdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>1/Jan/1993</t>
+  </si>
+  <si>
+    <t>checkFilters</t>
   </si>
 </sst>
 </file>
@@ -498,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,6 +628,44 @@
         <v>26</v>
       </c>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4">
+        <v>987654321</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <v>987654321</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented test case to check Saved Searches.
</commit_message>
<xml_diff>
--- a/resources/testdata.xlsx
+++ b/resources/testdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>checkFilters</t>
+  </si>
+  <si>
+    <t>checkSavedSearch</t>
   </si>
 </sst>
 </file>
@@ -501,14 +504,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
@@ -666,6 +670,44 @@
         <v>26</v>
       </c>
     </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5">
+        <v>987654321</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <v>987654321</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modified a bit to support round trip.
</commit_message>
<xml_diff>
--- a/resources/testdata.xlsx
+++ b/resources/testdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>checkSavedSearch</t>
+  </si>
+  <si>
+    <t>ToDate</t>
+  </si>
+  <si>
+    <t>20/12/2017</t>
+  </si>
+  <si>
+    <t>6/12/2017</t>
   </si>
 </sst>
 </file>
@@ -504,21 +513,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,25 +548,28 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -575,26 +588,29 @@
       <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>123456789</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1234567890</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -613,26 +629,29 @@
       <c r="F3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>987654321</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>987654321</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -651,26 +670,29 @@
       <c r="F4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>987654321</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>987654321</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -689,22 +711,25 @@
       <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>987654321</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>987654321</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>